<commit_message>
data tong hop 16/9
</commit_message>
<xml_diff>
--- a/Thuthapdulieu.xlsx
+++ b/Thuthapdulieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mai\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8143E9-BF38-4591-9C91-CA731BBA8F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F456795-4A99-40AF-98FB-4DCC2354AF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29890" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="625">
   <si>
     <t>id</t>
   </si>
@@ -1480,6 +1480,426 @@
   </si>
   <si>
     <t>000090</t>
+  </si>
+  <si>
+    <t>tap-can-binh-putin-hoi-dam-16632471999642079379827.jpg</t>
+  </si>
+  <si>
+    <t>Quang cảnh cuộc hội đàm của Tổng thống Nga Putin và Chủ tịch Trung Quốc Tập Cận Bình</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/15/tap-can-binh-putin-hoi-dam-16632471999642079379827.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/gap-ong-tap-ong-putin-cam-on-vi-lap-truong-can-bang-ve-ukraine-20220915200745443.htm</t>
+  </si>
+  <si>
+    <t>tap-can-binh-uzbekistan-16632318595661684551412.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chủ tịch Trung Quốc Tập Cận Bình (trái) và Tổng thống Uzbekistan Shavkat Mirziyoyev gặp nhau bên lề hội nghị thượng đỉnh SCO tại Samarkand, ngày 15-9 </t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/15/tap-can-binh-uzbekistan-16632318595661684551412.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/trung-quoc-va-uzbekistan-ky-thoa-thuan-hop-tac-dau-tu-15-ti-usd-20220915155244032.htm</t>
+  </si>
+  <si>
+    <t>screen-shot-2022-09-06-at-133102-16624458722901113389954.png</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/6/screen-shot-2022-09-06-at-133102-16624458722901113389954.png</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-putin-tham-du-tap-tran-chung-co-trung-quoc-tham-gia-20220906133731139.htm</t>
+  </si>
+  <si>
+    <t>biden-joe-1662432865503743809814.jpg</t>
+  </si>
+  <si>
+    <t>Tổng thống Mỹ Joe Biden</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/6/biden-joe-1662432865503743809814.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-biden-khong-xem-nga-la-nuoc-tai-tro-khung-bo-20220906095312915.htm</t>
+  </si>
+  <si>
+    <t>liz-truss-va-chong-1662435534917653268115.jpg</t>
+  </si>
+  <si>
+    <t>cuộc bỏ phiếu ở Trụ sở Đảng Bảo thủ</t>
+  </si>
+  <si>
+    <t>5/9/2022</t>
+  </si>
+  <si>
+    <t>Bà Liz Truss ăn mừng cùng chồng Hugh O'Leary khi được công bố trở thành tân thủ tướng</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/6/liz-truss-va-chong-1662435534917653268115.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/nu-hoang-anh-se-bo-nhiem-ba-liz-truss-lam-thu-tuong-chieu-6-9-20220906071357924.htm</t>
+  </si>
+  <si>
+    <t>2022-09-05t153938z749437738rc20bw9pwlmqrtrmadp3britain-politics-leadership-166241108105768004595.jpg</t>
+  </si>
+  <si>
+    <t>Tân thủ tướng Anh, bà Liz Truss</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/6/2022-09-05t153938z749437738rc20bw9pwlmqrtrmadp3britain-politics-leadership-166241108105768004595.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tin-the-gioi-6-9-ong-putin-duyet-hoc-thuyet-doi-ngoai-is-nhan-danh-bom-toa-dai-su-nga-20220906041253056.htm</t>
+  </si>
+  <si>
+    <t>putin-voi-chim-1662419365886142163094.jpg</t>
+  </si>
+  <si>
+    <t>tham gia một sự kiện với các nhà điểu học</t>
+  </si>
+  <si>
+    <t>Kamchatka</t>
+  </si>
+  <si>
+    <t>Tổng thống Vladimir Putin chụp ảnh lưu niệm ngày 5-9 khi tham gia một sự kiện với các nhà điểu học tại Kamchatka</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/6/putin-voi-chim-1662419365886142163094.jpg</t>
+  </si>
+  <si>
+    <t>2022-09-05t131852z2076156417rc21bw96y5akrtrmadp3britain-politics-leadership-1662393540257547012986.jpg</t>
+  </si>
+  <si>
+    <t>Bà Liz Truss vẫy chào sau khi chiến thắng cuộc bỏ phiếu để trở thành tân Thủ tướng Anh ngày 5-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/5/2022-09-05t131852z2076156417rc21bw96y5akrtrmadp3britain-politics-leadership-1662393540257547012986.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/cac-lanh-dao-chuc-mung-tan-thu-tuong-anh-20220905230134845.htm</t>
+  </si>
+  <si>
+    <t>liz-truss-1662371507931112468234.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/5/liz-truss-1662371507931112468234.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tan-thu-tuong-anh-liz-truss-nguoi-tung-dong-vai-ba-dam-thep-margaret-thatcher-2022090516575541.htm</t>
+  </si>
+  <si>
+    <t>liz-truss-o-moscow-16623715928071111326561.jpg</t>
+  </si>
+  <si>
+    <t>Ngoại trưởng Anh</t>
+  </si>
+  <si>
+    <t>chuyến thăm Matxcơva</t>
+  </si>
+  <si>
+    <t>10/2/2022</t>
+  </si>
+  <si>
+    <t>Bà Liz Truss ở Matxcơva, ngày 10-2-2022</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/5/liz-truss-o-moscow-16623715928071111326561.jpg</t>
+  </si>
+  <si>
+    <t>liz-truss-2-1662371706428366832096.jpg</t>
+  </si>
+  <si>
+    <t>Còn phải chờ xem tân Thủ tướng Liz Truss có mang lại sự ổn định cho chính trường Anh hay không</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/5/liz-truss-2-1662371706428366832096.jpg</t>
+  </si>
+  <si>
+    <t>afpcom-20220901-partners-068-aa01092022848700-highres-16623789092272112162378.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/5/afpcom-20220901-partners-068-aa01092022848700-highres-16623789092272112162378.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/nuoc-anh-co-tan-thu-tuong-20220905180640147.htm</t>
+  </si>
+  <si>
+    <t>tan-thu-tuong-anh-16623387274731371442077.jpg</t>
+  </si>
+  <si>
+    <t>Ngoại trưởng Liz Truss (trái) và cựu bộ trưởng tài chính Rishi Sunak</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/5/tan-thu-tuong-anh-16623387274731371442077.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tan-thu-tuong-anh-va-the-su-nong-bong-20220905074743709.htm</t>
+  </si>
+  <si>
+    <t>000091</t>
+  </si>
+  <si>
+    <t>000092</t>
+  </si>
+  <si>
+    <t>000093</t>
+  </si>
+  <si>
+    <t>000094</t>
+  </si>
+  <si>
+    <t>000095</t>
+  </si>
+  <si>
+    <t>000096</t>
+  </si>
+  <si>
+    <t>000097</t>
+  </si>
+  <si>
+    <t>000098</t>
+  </si>
+  <si>
+    <t>000099</t>
+  </si>
+  <si>
+    <t>000100</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>000102</t>
+  </si>
+  <si>
+    <t>000103</t>
+  </si>
+  <si>
+    <t>000104</t>
+  </si>
+  <si>
+    <t>1365341-1663306849706480451380.jpg</t>
+  </si>
+  <si>
+    <t>Chủ tịch Trung Quốc Tập Cận Bình (trái) và Tổng thống Nga Vladimir Putin</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/1365341-1663306849706480451380.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tass-ong-tap-va-ong-putin-tro-chuyen-binh-thuong-khong-deo-khau-trang-20220916130226199.htm</t>
+  </si>
+  <si>
+    <t>putin-tap-1663288936795901602946-16633105779532049001225.jpg</t>
+  </si>
+  <si>
+    <t>Tổng thống Vladimir Putin và Chủ tịch Tập Cận Bình ngồi cách xa nhau trong cuộc gặp song phương bên lề thượng đỉnh SCO ở Uzbekistan ngày 15-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/putin-tap-1663288936795901602946-16633105779532049001225.jpg</t>
+  </si>
+  <si>
+    <t>2022-09-16t061649z1035245409rc25iw9s8ml8rtrmadp3uzbekistan-sco-16633104396692113763349.jpg</t>
+  </si>
+  <si>
+    <t>một cuộc họp hội nghị thượng đỉnh của Tổ chức Hợp tác Thượng Hải (SCO)</t>
+  </si>
+  <si>
+    <t>16/9/2022</t>
+  </si>
+  <si>
+    <t>Lãnh đạo các nước thành viên Tổ chức Hợp tác Thượng Hải (SCO) trong một cuộc họp hẹp ở Samarkand, Uzbekistan ngày 16-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/2022-09-16t061649z1035245409rc25iw9s8ml8rtrmadp3uzbekistan-sco-16633104396692113763349.jpg</t>
+  </si>
+  <si>
+    <t>putin-tap-1663288936795901602946.jpg</t>
+  </si>
+  <si>
+    <t>Tổng thống Nga Vladimir Putin (bìa trái) gặp Chủ tịch Trung Quốc Tập Cận Bình bên lề hội nghị thượng đỉnh SCO ở Uzbekistan vào ngày 15-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/putin-tap-1663288936795901602946.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/mat-tran-chong-phuong-tay-o-uzbekistan-20220916074558429.htm</t>
+  </si>
+  <si>
+    <t>tap-putin-16632866301671178504273.jpg</t>
+  </si>
+  <si>
+    <t>Ảnh ghép cho thấy Tổng thống Nga Vladimir Putin (trái) và Chủ tịch Trung Quốc Tập Cận Bình trong cuộc gặp bên lề hội nghị thượng đỉnh của SCO ở Samarkand, Uzbekistan ngày 15-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/tap-putin-16632866301671178504273.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-tap-khong-quoc-gia-nao-co-quyen-lam-nguoi-phan-xu-ve-van-de-dai-loan-20220916064715016.htm</t>
+  </si>
+  <si>
+    <t>32hy8j7-highres-16626836653231240712451.jpg</t>
+  </si>
+  <si>
+    <t>hội nghị thượng đỉnh G7</t>
+  </si>
+  <si>
+    <t>11/6/2021</t>
+  </si>
+  <si>
+    <t>Cornwall</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth II chụp ảnh cùng các lãnh đạo thế giới tại Anh vào tháng 6-2021</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/32hy8j7-highres-16626836653231240712451.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/lanh-dao-the-gioi-tiec-thuong-va-ca-ngoi-nu-hoang-anh-20220909073936491.htm</t>
+  </si>
+  <si>
+    <t>32hy8kt-highres-1662683804651672983270.jpg</t>
+  </si>
+  <si>
+    <t>chuyến công du Vatican</t>
+  </si>
+  <si>
+    <t>3/4/2014</t>
+  </si>
+  <si>
+    <t>Vatican</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth II bắt tay Giáo hoàng Francis tại Vatican năm 2014</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/32hy8kt-highres-1662683804651672983270.jpg</t>
+  </si>
+  <si>
+    <t>thai-tu-charles-1662691648508697562842.jpg</t>
+  </si>
+  <si>
+    <t>lễ khai mạc Quốc hội</t>
+  </si>
+  <si>
+    <t>19/12/2019</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Anh Elizabeth II và Thái tử Charles, thân vương Xứ Wales</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/thai-tu-charles-1662691648508697562842.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/vua-charles-iii-chia-se-ve-giay-phut-nu-hoang-bang-ha-khoanh-khac-buon-nhat-cuoc-doi-toi-20220909090737266.htm</t>
+  </si>
+  <si>
+    <t>2022-09-08t191538z533084643rc2obw9qew2zrtrmadp3britain-royals-queen-16626738914421086763583.jpg</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth II chờ tiếp kiến tân Thủ tướng Anh Liz Truss tại lâu đài Balmoral ngày 6-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/2022-09-08t191538z533084643rc2obw9qew2zrtrmadp3britain-royals-queen-16626738914421086763583.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ke-hoach-tang-le-da-duoc-chinh-nu-hoang-anh-thong-qua-20220909050051765.htm</t>
+  </si>
+  <si>
+    <t>2022-09-08t173805z409843283rc2v7l7y9il0rtrmadp3britain-royals-queen-1662673973438478989573.jpg</t>
+  </si>
+  <si>
+    <t>triển lãm hoa Chelsea</t>
+  </si>
+  <si>
+    <t>24/5/2010</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth băng hà rạng sáng ngày 9-9, giờ Việt Nam</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/2022-09-08t173805z409843283rc2v7l7y9il0rtrmadp3britain-royals-queen-1662673973438478989573.jpg</t>
+  </si>
+  <si>
+    <t>2022-09-08t173647z38271561rc2tlu9k2tw0rtrmadp3britain-royals-queen-1662674011648476926570.jpg</t>
+  </si>
+  <si>
+    <t>cuộc thi Platinum Jubilee Pageant và lễ bế mạc đại lễ bạch kim</t>
+  </si>
+  <si>
+    <t>5/6/2022</t>
+  </si>
+  <si>
+    <t>Thái tử Charles đứng cạnh Nữ hoàng Elizabeth đệ nhị tại một sự kiện vào tháng 6-2022</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/2022-09-08t173647z38271561rc2tlu9k2tw0rtrmadp3britain-royals-queen-1662674011648476926570.jpg</t>
+  </si>
+  <si>
+    <t>000105</t>
+  </si>
+  <si>
+    <t>000106</t>
+  </si>
+  <si>
+    <t>000107</t>
+  </si>
+  <si>
+    <t>000108</t>
+  </si>
+  <si>
+    <t>000109</t>
+  </si>
+  <si>
+    <t>000110</t>
+  </si>
+  <si>
+    <t>000111</t>
+  </si>
+  <si>
+    <t>000112</t>
+  </si>
+  <si>
+    <t>000113</t>
+  </si>
+  <si>
+    <t>000114</t>
+  </si>
+  <si>
+    <t>000115</t>
+  </si>
+  <si>
+    <t>000116</t>
+  </si>
+  <si>
+    <t>000117</t>
+  </si>
+  <si>
+    <t>000118</t>
+  </si>
+  <si>
+    <t>000119</t>
+  </si>
+  <si>
+    <t>000120</t>
+  </si>
+  <si>
+    <t>000121</t>
+  </si>
+  <si>
+    <t>000122</t>
+  </si>
+  <si>
+    <t>000123</t>
+  </si>
+  <si>
+    <t>000124</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +2025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1620,8 +2040,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1635,6 +2053,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1856,8 +2277,8 @@
   </sheetPr>
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -1953,10 +2374,10 @@
       <c r="L2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="5" t="s">
@@ -1993,10 +2414,10 @@
       <c r="L3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="15"/>
+      <c r="N3" s="29"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="5" t="s">
@@ -2033,10 +2454,10 @@
       <c r="L4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="15"/>
+      <c r="N4" s="29"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="5" t="s">
@@ -2073,10 +2494,10 @@
       <c r="L5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="15"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
@@ -2113,10 +2534,10 @@
       <c r="L6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="N6" s="15"/>
+      <c r="N6" s="29"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="5" t="s">
@@ -2153,10 +2574,10 @@
       <c r="L7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="15"/>
+      <c r="N7" s="29"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="5" t="s">
@@ -2193,10 +2614,10 @@
       <c r="L8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="15"/>
+      <c r="N8" s="29"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="5" t="s">
@@ -2233,10 +2654,10 @@
       <c r="L9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N9" s="15"/>
+      <c r="N9" s="29"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="5" t="s">
@@ -2273,10 +2694,10 @@
       <c r="L10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="15"/>
+      <c r="N10" s="29"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="5" t="s">
@@ -2313,10 +2734,10 @@
       <c r="L11" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N11" s="15"/>
+      <c r="N11" s="29"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="5" t="s">
@@ -2353,10 +2774,10 @@
       <c r="L12" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="M12" s="14" t="s">
+      <c r="M12" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N12" s="15"/>
+      <c r="N12" s="29"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="5" t="s">
@@ -2393,10 +2814,10 @@
       <c r="L13" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="N13" s="15"/>
+      <c r="N13" s="29"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="5" t="s">
@@ -2433,10 +2854,10 @@
       <c r="L14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="29"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="5" t="s">
@@ -2473,10 +2894,10 @@
       <c r="L15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="15"/>
+      <c r="N15" s="29"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="5" t="s">
@@ -2513,10 +2934,10 @@
       <c r="L16" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="N16" s="15"/>
+      <c r="N16" s="29"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="5" t="s">
@@ -2553,10 +2974,10 @@
       <c r="L17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N17" s="15"/>
+      <c r="N17" s="29"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="5" t="s">
@@ -2593,10 +3014,10 @@
       <c r="L18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="29"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="5" t="s">
@@ -2633,10 +3054,10 @@
       <c r="L19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="15"/>
+      <c r="N19" s="29"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="5" t="s">
@@ -2673,10 +3094,10 @@
       <c r="L20" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="15"/>
+      <c r="N20" s="29"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
@@ -2713,10 +3134,10 @@
       <c r="L21" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N21" s="15"/>
+      <c r="N21" s="29"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="5" t="s">
@@ -2753,10 +3174,10 @@
       <c r="L22" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N22" s="15"/>
+      <c r="N22" s="29"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="5" t="s">
@@ -2793,10 +3214,10 @@
       <c r="L23" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N23" s="15"/>
+      <c r="N23" s="29"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="5" t="s">
@@ -2833,10 +3254,10 @@
       <c r="L24" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N24" s="15"/>
+      <c r="N24" s="29"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="5" t="s">
@@ -2873,10 +3294,10 @@
       <c r="L25" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N25" s="15"/>
+      <c r="N25" s="29"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="5" t="s">
@@ -2913,10 +3334,10 @@
       <c r="L26" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="M26" s="14" t="s">
+      <c r="M26" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="N26" s="15"/>
+      <c r="N26" s="29"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="5" t="s">
@@ -2953,10 +3374,10 @@
       <c r="L27" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="N27" s="15"/>
+      <c r="N27" s="29"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="5" t="s">
@@ -2993,10 +3414,10 @@
       <c r="L28" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="M28" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="N28" s="15"/>
+      <c r="N28" s="29"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="5" t="s">
@@ -3033,10 +3454,10 @@
       <c r="L29" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="M29" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="N29" s="15"/>
+      <c r="N29" s="29"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="5" t="s">
@@ -3073,10 +3494,10 @@
       <c r="L30" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="M30" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="N30" s="15"/>
+      <c r="N30" s="29"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="5" t="s">
@@ -3113,10 +3534,10 @@
       <c r="L31" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="M31" s="14" t="s">
+      <c r="M31" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="N31" s="15"/>
+      <c r="N31" s="29"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="5" t="s">
@@ -4007,7 +4428,7 @@
       <c r="B56" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -4016,7 +4437,7 @@
       <c r="E56" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="15" t="s">
         <v>289</v>
       </c>
       <c r="G56" s="10" t="s">
@@ -4025,7 +4446,7 @@
       <c r="H56" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="I56" s="16"/>
+      <c r="I56" s="14"/>
       <c r="J56" s="10" t="s">
         <v>292</v>
       </c>
@@ -4038,7 +4459,7 @@
       <c r="M56" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="N56" s="16"/>
+      <c r="N56" s="14"/>
     </row>
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A57" s="6" t="s">
@@ -4065,7 +4486,7 @@
       <c r="H57" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="I57" s="16"/>
+      <c r="I57" s="14"/>
       <c r="J57" s="10" t="s">
         <v>300</v>
       </c>
@@ -4089,13 +4510,13 @@
       <c r="B58" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D58" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E58" s="16" t="s">
         <v>306</v>
       </c>
       <c r="F58" s="11" t="s">
@@ -4107,7 +4528,7 @@
       <c r="H58" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="I58" s="16"/>
+      <c r="I58" s="14"/>
       <c r="J58" s="10" t="s">
         <v>22</v>
       </c>
@@ -4120,7 +4541,7 @@
       <c r="M58" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="N58" s="16"/>
+      <c r="N58" s="14"/>
     </row>
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A59" s="6" t="s">
@@ -4135,7 +4556,7 @@
       <c r="D59" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E59" s="16" t="s">
         <v>306</v>
       </c>
       <c r="F59" s="11" t="s">
@@ -4147,7 +4568,7 @@
       <c r="H59" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="I59" s="16"/>
+      <c r="I59" s="14"/>
       <c r="J59" s="10" t="s">
         <v>22</v>
       </c>
@@ -4160,7 +4581,7 @@
       <c r="M59" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="N59" s="16"/>
+      <c r="N59" s="14"/>
     </row>
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A60" s="6" t="s">
@@ -4175,7 +4596,7 @@
       <c r="D60" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E60" s="18" t="s">
+      <c r="E60" s="16" t="s">
         <v>317</v>
       </c>
       <c r="F60" s="11" t="s">
@@ -4187,7 +4608,7 @@
       <c r="H60" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="I60" s="16"/>
+      <c r="I60" s="14"/>
       <c r="J60" s="10" t="s">
         <v>36</v>
       </c>
@@ -4200,7 +4621,7 @@
       <c r="M60" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="N60" s="16"/>
+      <c r="N60" s="14"/>
     </row>
     <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A61" s="6" t="s">
@@ -4215,7 +4636,7 @@
       <c r="D61" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="18" t="s">
+      <c r="E61" s="16" t="s">
         <v>324</v>
       </c>
       <c r="F61" s="11" t="s">
@@ -4227,7 +4648,7 @@
       <c r="H61" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I61" s="16"/>
+      <c r="I61" s="14"/>
       <c r="J61" s="10" t="s">
         <v>22</v>
       </c>
@@ -4240,7 +4661,7 @@
       <c r="M61" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="N61" s="16"/>
+      <c r="N61" s="14"/>
     </row>
     <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A62" s="6" t="s">
@@ -4255,19 +4676,19 @@
       <c r="D62" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="H62" s="19" t="s">
+      <c r="H62" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="I62" s="16"/>
+      <c r="I62" s="14"/>
       <c r="J62" s="10" t="s">
         <v>36</v>
       </c>
@@ -4280,7 +4701,7 @@
       <c r="M62" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="N62" s="16"/>
+      <c r="N62" s="14"/>
     </row>
     <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A63" s="6" t="s">
@@ -4295,19 +4716,19 @@
       <c r="D63" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F63" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="H63" s="19" t="s">
+      <c r="H63" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="I63" s="16"/>
+      <c r="I63" s="14"/>
       <c r="J63" s="10" t="s">
         <v>36</v>
       </c>
@@ -4320,13 +4741,13 @@
       <c r="M63" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="N63" s="16"/>
+      <c r="N63" s="14"/>
     </row>
     <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A64" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="14" t="s">
         <v>333</v>
       </c>
       <c r="C64" s="10" t="s">
@@ -4335,38 +4756,38 @@
       <c r="D64" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="E64" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="F64" s="21" t="s">
+      <c r="F64" s="19" t="s">
         <v>334</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="H64" s="16" t="s">
+      <c r="H64" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="I64" s="16"/>
+      <c r="I64" s="14"/>
       <c r="J64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K64" s="16" t="s">
+      <c r="K64" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="L64" s="16" t="s">
+      <c r="L64" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="M64" s="16" t="s">
+      <c r="M64" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="N64" s="16"/>
+      <c r="N64" s="14"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A65" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="14" t="s">
         <v>339</v>
       </c>
       <c r="C65" s="10" t="s">
@@ -4375,10 +4796,10 @@
       <c r="D65" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E65" s="18" t="s">
+      <c r="E65" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="F65" s="21" t="s">
+      <c r="F65" s="19" t="s">
         <v>341</v>
       </c>
       <c r="G65" s="10" t="s">
@@ -4387,26 +4808,26 @@
       <c r="H65" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="I65" s="16"/>
+      <c r="I65" s="14"/>
       <c r="J65" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="K65" s="16" t="s">
+      <c r="K65" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="L65" s="16" t="s">
+      <c r="L65" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="M65" s="16" t="s">
+      <c r="M65" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="N65" s="16"/>
+      <c r="N65" s="14"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A66" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="14" t="s">
         <v>339</v>
       </c>
       <c r="C66" s="10" t="s">
@@ -4415,10 +4836,10 @@
       <c r="D66" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E66" s="18" t="s">
+      <c r="E66" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" s="19" t="s">
         <v>341</v>
       </c>
       <c r="G66" s="10" t="s">
@@ -4427,52 +4848,52 @@
       <c r="H66" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="I66" s="16"/>
+      <c r="I66" s="14"/>
       <c r="J66" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="K66" s="16" t="s">
+      <c r="K66" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="L66" s="16" t="s">
+      <c r="L66" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="M66" s="16" t="s">
+      <c r="M66" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="N66" s="16"/>
+      <c r="N66" s="14"/>
     </row>
     <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A67" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="C67" s="18" t="s">
+      <c r="C67" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E67" s="19"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="16"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="14"/>
       <c r="J67" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K67" s="16" t="s">
+      <c r="K67" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="L67" s="16" t="s">
+      <c r="L67" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="M67" s="16" t="s">
+      <c r="M67" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="N67" s="16" t="s">
+      <c r="N67" s="14" t="s">
         <v>352</v>
       </c>
     </row>
@@ -4480,273 +4901,273 @@
       <c r="A68" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D68" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="18" t="s">
+      <c r="E68" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F68" s="21" t="s">
+      <c r="F68" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="G68" s="18" t="s">
+      <c r="G68" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="H68" s="18" t="s">
+      <c r="H68" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="I68" s="16"/>
+      <c r="I68" s="14"/>
       <c r="J68" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K68" s="16" t="s">
+      <c r="K68" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="L68" s="16" t="s">
+      <c r="L68" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="M68" s="16" t="s">
+      <c r="M68" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="N68" s="16"/>
+      <c r="N68" s="14"/>
     </row>
     <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A69" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="D69" s="18" t="s">
+      <c r="D69" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E69" s="18" t="s">
+      <c r="E69" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F69" s="21" t="s">
+      <c r="F69" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="G69" s="18" t="s">
+      <c r="G69" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="H69" s="18" t="s">
+      <c r="H69" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="I69" s="16"/>
+      <c r="I69" s="14"/>
       <c r="J69" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K69" s="16" t="s">
+      <c r="K69" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="L69" s="16" t="s">
+      <c r="L69" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="M69" s="16" t="s">
+      <c r="M69" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="N69" s="16"/>
+      <c r="N69" s="14"/>
     </row>
     <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A70" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C70" s="18" t="s">
+      <c r="C70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="E70" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F70" s="21" t="s">
+      <c r="F70" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="G70" s="18" t="s">
+      <c r="G70" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="H70" s="18" t="s">
+      <c r="H70" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="I70" s="16"/>
+      <c r="I70" s="14"/>
       <c r="J70" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K70" s="16" t="s">
+      <c r="K70" s="14" t="s">
         <v>358</v>
       </c>
-      <c r="L70" s="16" t="s">
+      <c r="L70" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="M70" s="16" t="s">
+      <c r="M70" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="N70" s="16"/>
+      <c r="N70" s="14"/>
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A71" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C71" s="18" t="s">
+      <c r="C71" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D71" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E71" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F71" s="21" t="s">
+      <c r="F71" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="G71" s="18" t="s">
+      <c r="G71" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="H71" s="18" t="s">
+      <c r="H71" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="I71" s="16"/>
+      <c r="I71" s="14"/>
       <c r="J71" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K71" s="16" t="s">
+      <c r="K71" s="14" t="s">
         <v>358</v>
       </c>
-      <c r="L71" s="16" t="s">
+      <c r="L71" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="M71" s="16" t="s">
+      <c r="M71" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="N71" s="16"/>
+      <c r="N71" s="14"/>
     </row>
     <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A72" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="C72" s="18" t="s">
+      <c r="C72" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D72" s="18" t="s">
+      <c r="D72" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E72" s="18" t="s">
+      <c r="E72" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="F72" s="21" t="s">
+      <c r="F72" s="19" t="s">
         <v>363</v>
       </c>
-      <c r="G72" s="18" t="s">
+      <c r="G72" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="H72" s="18" t="s">
+      <c r="H72" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="I72" s="16"/>
+      <c r="I72" s="14"/>
       <c r="J72" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K72" s="16" t="s">
+      <c r="K72" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="L72" s="16" t="s">
+      <c r="L72" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="M72" s="16" t="s">
+      <c r="M72" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="N72" s="16"/>
+      <c r="N72" s="14"/>
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A73" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="B73" s="19" t="s">
+      <c r="B73" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D73" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="E73" s="18" t="s">
+      <c r="E73" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="F73" s="21" t="s">
+      <c r="F73" s="19" t="s">
         <v>363</v>
       </c>
-      <c r="G73" s="18" t="s">
+      <c r="G73" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="H73" s="18" t="s">
+      <c r="H73" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="I73" s="16"/>
+      <c r="I73" s="14"/>
       <c r="J73" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K73" s="16" t="s">
+      <c r="K73" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="L73" s="16" t="s">
+      <c r="L73" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="M73" s="16" t="s">
+      <c r="M73" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="N73" s="16"/>
+      <c r="N73" s="14"/>
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A74" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D74" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
       <c r="J74" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="K74" s="16" t="s">
+      <c r="K74" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="L74" s="22" t="s">
+      <c r="L74" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="M74" s="16" t="s">
+      <c r="M74" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="N74" s="19" t="s">
+      <c r="N74" s="17" t="s">
         <v>352</v>
       </c>
     </row>
@@ -4754,379 +5175,379 @@
       <c r="A75" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D75" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="E75" s="18" t="s">
+      <c r="E75" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="F75" s="21" t="s">
+      <c r="F75" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G75" s="18" t="s">
+      <c r="G75" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="H75" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I75" s="16"/>
+      <c r="I75" s="14"/>
       <c r="J75" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K75" s="19" t="s">
+      <c r="K75" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="L75" s="19" t="s">
+      <c r="L75" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="M75" s="16" t="s">
+      <c r="M75" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="N75" s="16"/>
+      <c r="N75" s="14"/>
     </row>
     <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A76" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="C76" s="18" t="s">
+      <c r="C76" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="D76" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E76" s="18" t="s">
+      <c r="E76" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="F76" s="21" t="s">
+      <c r="F76" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="G76" s="18" t="s">
+      <c r="G76" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="H76" s="18" t="s">
+      <c r="H76" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I76" s="16"/>
+      <c r="I76" s="14"/>
       <c r="J76" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="K76" s="19" t="s">
+      <c r="K76" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="L76" s="19" t="s">
+      <c r="L76" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="M76" s="16" t="s">
+      <c r="M76" s="14" t="s">
         <v>385</v>
       </c>
-      <c r="N76" s="16"/>
+      <c r="N76" s="14"/>
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A77" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="C77" s="18" t="s">
+      <c r="C77" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="D77" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E77" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F77" s="21" t="s">
+      <c r="F77" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="G77" s="18" t="s">
+      <c r="G77" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="H77" s="18" t="s">
+      <c r="H77" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I77" s="16"/>
-      <c r="J77" s="23" t="s">
+      <c r="I77" s="14"/>
+      <c r="J77" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K77" s="16" t="s">
+      <c r="K77" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="L77" s="16" t="s">
+      <c r="L77" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="M77" s="16" t="s">
+      <c r="M77" s="14" t="s">
         <v>389</v>
       </c>
-      <c r="N77" s="16"/>
+      <c r="N77" s="14"/>
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A78" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C78" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D78" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="E78" s="18" t="s">
+      <c r="E78" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="F78" s="20" t="s">
+      <c r="F78" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="G78" s="18" t="s">
+      <c r="G78" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="H78" s="18" t="s">
+      <c r="H78" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I78" s="16"/>
+      <c r="I78" s="14"/>
       <c r="J78" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="K78" s="16" t="s">
+      <c r="K78" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="L78" s="19" t="s">
+      <c r="L78" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="M78" s="16" t="s">
+      <c r="M78" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="N78" s="16"/>
+      <c r="N78" s="14"/>
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A79" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D79" s="18" t="s">
+      <c r="D79" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E79" s="18" t="s">
+      <c r="E79" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F79" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="G79" s="18" t="s">
+      <c r="G79" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="H79" s="18" t="s">
+      <c r="H79" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I79" s="16"/>
+      <c r="I79" s="14"/>
       <c r="J79" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="K79" s="16" t="s">
+      <c r="K79" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="L79" s="19" t="s">
+      <c r="L79" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="M79" s="16" t="s">
+      <c r="M79" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="N79" s="16"/>
+      <c r="N79" s="14"/>
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A80" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D80" s="18" t="s">
+      <c r="D80" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E80" s="18" t="s">
+      <c r="E80" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="F80" s="20" t="s">
+      <c r="F80" s="18" t="s">
         <v>399</v>
       </c>
-      <c r="G80" s="18" t="s">
+      <c r="G80" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="H80" s="18" t="s">
+      <c r="H80" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I80" s="16"/>
+      <c r="I80" s="14"/>
       <c r="J80" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K80" s="16" t="s">
+      <c r="K80" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="L80" s="16" t="s">
+      <c r="L80" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="M80" s="16" t="s">
+      <c r="M80" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="N80" s="16"/>
+      <c r="N80" s="14"/>
     </row>
     <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A81" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="C81" s="18" t="s">
+      <c r="C81" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D81" s="18" t="s">
+      <c r="D81" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E81" s="18" t="s">
+      <c r="E81" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="F81" s="20" t="s">
+      <c r="F81" s="18" t="s">
         <v>405</v>
       </c>
-      <c r="G81" s="18" t="s">
+      <c r="G81" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="H81" s="18" t="s">
+      <c r="H81" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="I81" s="16"/>
+      <c r="I81" s="14"/>
       <c r="J81" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K81" s="16" t="s">
+      <c r="K81" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="L81" s="19" t="s">
+      <c r="L81" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="M81" s="16" t="s">
+      <c r="M81" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="N81" s="16"/>
+      <c r="N81" s="14"/>
     </row>
     <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A82" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D82" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="E82" s="18" t="s">
+      <c r="E82" s="16" t="s">
         <v>410</v>
       </c>
-      <c r="F82" s="20" t="s">
+      <c r="F82" s="18" t="s">
         <v>411</v>
       </c>
-      <c r="G82" s="18" t="s">
+      <c r="G82" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="H82" s="18" t="s">
+      <c r="H82" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="I82" s="16"/>
+      <c r="I82" s="14"/>
       <c r="J82" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K82" s="16" t="s">
+      <c r="K82" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="L82" s="16" t="s">
+      <c r="L82" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="M82" s="16" t="s">
+      <c r="M82" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="N82" s="16"/>
+      <c r="N82" s="14"/>
     </row>
     <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A83" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="D83" s="18" t="s">
+      <c r="D83" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E83" s="19" t="s">
+      <c r="E83" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="F83" s="21" t="s">
+      <c r="F83" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="G83" s="16" t="s">
+      <c r="G83" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="H83" s="16" t="s">
+      <c r="H83" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="I83" s="16"/>
+      <c r="I83" s="14"/>
       <c r="J83" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K83" s="19" t="s">
+      <c r="K83" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="L83" s="16" t="s">
+      <c r="L83" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="M83" s="16" t="s">
+      <c r="M83" s="14" t="s">
         <v>418</v>
       </c>
-      <c r="N83" s="16"/>
+      <c r="N83" s="14"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A84" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="C84" s="25" t="s">
+      <c r="C84" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D84" s="18" t="s">
+      <c r="D84" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="E84" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="F84" s="21" t="s">
+      <c r="F84" s="19" t="s">
         <v>158</v>
       </c>
       <c r="G84" s="10" t="s">
@@ -5135,220 +5556,220 @@
       <c r="H84" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I84" s="16"/>
+      <c r="I84" s="14"/>
       <c r="J84" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K84" s="19" t="s">
+      <c r="K84" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="L84" s="16" t="s">
+      <c r="L84" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="M84" s="16" t="s">
+      <c r="M84" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="N84" s="16"/>
+      <c r="N84" s="14"/>
     </row>
     <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A85" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="14" t="s">
         <v>423</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D85" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="F85" s="20" t="s">
+      <c r="F85" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G85" s="19" t="s">
+      <c r="G85" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H85" s="19" t="s">
+      <c r="H85" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="I85" s="16"/>
+      <c r="I85" s="14"/>
       <c r="J85" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K85" s="16" t="s">
+      <c r="K85" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="L85" s="16" t="s">
+      <c r="L85" s="14" t="s">
         <v>425</v>
       </c>
-      <c r="M85" s="16" t="s">
+      <c r="M85" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="N85" s="16"/>
+      <c r="N85" s="14"/>
     </row>
     <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A86" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D86" s="18" t="s">
+      <c r="D86" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="F86" s="20" t="s">
+      <c r="F86" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G86" s="19" t="s">
+      <c r="G86" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H86" s="19" t="s">
+      <c r="H86" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="I86" s="16"/>
+      <c r="I86" s="14"/>
       <c r="J86" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K86" s="16" t="s">
+      <c r="K86" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="L86" s="16" t="s">
+      <c r="L86" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="M86" s="16" t="s">
+      <c r="M86" s="14" t="s">
         <v>429</v>
       </c>
-      <c r="N86" s="16"/>
+      <c r="N86" s="14"/>
     </row>
     <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A87" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="D87" s="18" t="s">
+      <c r="D87" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E87" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F87" s="20" t="s">
+      <c r="F87" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="G87" s="19" t="s">
+      <c r="G87" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="H87" s="19" t="s">
+      <c r="H87" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="I87" s="16"/>
-      <c r="J87" s="19" t="s">
+      <c r="I87" s="14"/>
+      <c r="J87" s="17" t="s">
         <v>431</v>
       </c>
-      <c r="K87" s="16" t="s">
+      <c r="K87" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="L87" s="16" t="s">
+      <c r="L87" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="M87" s="16" t="s">
+      <c r="M87" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="N87" s="16"/>
+      <c r="N87" s="14"/>
     </row>
     <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A88" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="14" t="s">
         <v>435</v>
       </c>
-      <c r="C88" s="24" t="s">
+      <c r="C88" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="D88" s="18" t="s">
+      <c r="D88" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F88" s="20" t="s">
+      <c r="F88" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="G88" s="19" t="s">
+      <c r="G88" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="H88" s="19" t="s">
+      <c r="H88" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="I88" s="16"/>
+      <c r="I88" s="14"/>
       <c r="J88" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K88" s="16" t="s">
+      <c r="K88" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="L88" s="16" t="s">
+      <c r="L88" s="14" t="s">
         <v>437</v>
       </c>
-      <c r="M88" s="16" t="s">
+      <c r="M88" s="14" t="s">
         <v>438</v>
       </c>
-      <c r="N88" s="16"/>
+      <c r="N88" s="14"/>
     </row>
     <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A89" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="C89" s="24" t="s">
+      <c r="C89" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D89" s="18" t="s">
+      <c r="D89" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E89" s="19" t="s">
+      <c r="E89" s="17" t="s">
         <v>440</v>
       </c>
-      <c r="F89" s="20" t="s">
+      <c r="F89" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="G89" s="19" t="s">
+      <c r="G89" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H89" s="19" t="s">
+      <c r="H89" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="I89" s="16"/>
+      <c r="I89" s="14"/>
       <c r="J89" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K89" s="16" t="s">
+      <c r="K89" s="14" t="s">
         <v>441</v>
       </c>
-      <c r="L89" s="16" t="s">
+      <c r="L89" s="14" t="s">
         <v>442</v>
       </c>
-      <c r="M89" s="16" t="s">
+      <c r="M89" s="14" t="s">
         <v>443</v>
       </c>
-      <c r="N89" s="16"/>
+      <c r="N89" s="14"/>
     </row>
     <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A90" s="6" t="s">
@@ -5357,25 +5778,25 @@
       <c r="B90" t="s">
         <v>444</v>
       </c>
-      <c r="C90" s="24" t="s">
+      <c r="C90" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D90" s="18" t="s">
+      <c r="D90" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E90" s="26" t="s">
+      <c r="E90" s="24" t="s">
         <v>445</v>
       </c>
-      <c r="F90" s="27" t="s">
+      <c r="F90" s="25" t="s">
         <v>446</v>
       </c>
-      <c r="G90" s="26" t="s">
+      <c r="G90" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="H90" s="26" t="s">
+      <c r="H90" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="J90" s="28" t="s">
+      <c r="J90" s="26" t="s">
         <v>36</v>
       </c>
       <c r="K90" t="s">
@@ -5395,25 +5816,25 @@
       <c r="B91" t="s">
         <v>444</v>
       </c>
-      <c r="C91" s="24" t="s">
+      <c r="C91" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D91" s="18" t="s">
+      <c r="D91" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="E91" s="26" t="s">
+      <c r="E91" s="24" t="s">
         <v>445</v>
       </c>
-      <c r="F91" s="27" t="s">
+      <c r="F91" s="25" t="s">
         <v>446</v>
       </c>
-      <c r="G91" s="26" t="s">
+      <c r="G91" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="H91" s="26" t="s">
+      <c r="H91" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="J91" s="28" t="s">
+      <c r="J91" s="26" t="s">
         <v>36</v>
       </c>
       <c r="K91" t="s">
@@ -5426,43 +5847,1238 @@
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="92" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A92" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K92" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A93" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K93" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A94" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J94" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K94" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="M94" s="14" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A95" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K95" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="N95" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A96" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J96" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K96" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="L96" s="14" t="s">
+        <v>498</v>
+      </c>
+      <c r="M96" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="N96" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A97" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J97" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K97" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="L97" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="M97" s="14" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A98" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J98" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K98" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="L98" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="M98" s="14" t="s">
+        <v>509</v>
+      </c>
+      <c r="N98" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A99" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="F99" s="27" t="s">
+        <v>502</v>
+      </c>
+      <c r="G99" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="H99" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J99" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K99" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="L99" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="M99" s="14" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A100" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E100" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="F100" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K100" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="L100" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="M100" s="14" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A101" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>519</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J101" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K101" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="L101" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="M101" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="N101" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A102" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="E102" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="F102" s="27" t="s">
+        <v>525</v>
+      </c>
+      <c r="G102" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H102" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J102" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K102" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="L102" s="14" t="s">
+        <v>527</v>
+      </c>
+      <c r="M102" s="14" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A103" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="J103" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K103" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="L103" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="M103" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="N103" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A104" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="J104" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K104" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="L104" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="M104" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="N104" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A105" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>534</v>
+      </c>
+      <c r="C105" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="J105" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K105" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="L105" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="M105" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="N105" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A106" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G106" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H106" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J106" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="K106" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="L106" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="M106" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A107" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F107" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J107" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="K107" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="L107" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="M107" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A108" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F108" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G108" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H108" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J108" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K108" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="L108" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="M108" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A109" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F109" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G109" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H109" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K109" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="L109" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="M109" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A110" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J110" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K110" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="L110" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="M110" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A111" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C111" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K111" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="L111" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="M111" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A112" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="C112" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F112" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G112" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J112" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K112" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="L112" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="M112" s="14" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A113" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="C113" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H113" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J113" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K113" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="L113" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="M113" s="14" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A114" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="C114" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G114" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H114" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J114" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K114" s="14" t="s">
+        <v>569</v>
+      </c>
+      <c r="L114" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="M114" s="14" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A115" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F115" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H115" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J115" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K115" s="14" t="s">
+        <v>569</v>
+      </c>
+      <c r="L115" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="M115" s="14" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A116" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="G116" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="H116" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J116" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K116" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="L116" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="M116" s="14" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A117" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D117" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="F117" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="G117" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="H117" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J117" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K117" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="L117" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="M117" s="14" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A118" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="C118" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="F118" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="G118" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="H118" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J118" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K118" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="L118" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="M118" s="14" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A119" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="C119" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="F119" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="G119" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="H119" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="J119" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K119" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="L119" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="M119" s="14" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A120" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="C120" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="F120" s="15" t="s">
+        <v>587</v>
+      </c>
+      <c r="G120" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H120" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J120" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K120" s="14" t="s">
+        <v>588</v>
+      </c>
+      <c r="L120" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="M120" s="14" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A121" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="C121" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D121" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="F121" s="15" t="s">
+        <v>587</v>
+      </c>
+      <c r="G121" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H121" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J121" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K121" s="14" t="s">
+        <v>588</v>
+      </c>
+      <c r="L121" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="M121" s="14" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A122" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>591</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E122" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F122" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="G122" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="H122" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="J122" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K122" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="L122" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="M122" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A123" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="C123" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E123" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="F123" s="15" t="s">
+        <v>597</v>
+      </c>
+      <c r="G123" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H123" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J123" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K123" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="L123" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="M123" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A124" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="C124" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E124" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="F124" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="G124" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H124" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J124" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K124" s="14" t="s">
+        <v>603</v>
+      </c>
+      <c r="L124" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="M124" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A125" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="C125" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E125" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="F125" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="G125" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H125" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J125" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K125" s="14" t="s">
+        <v>603</v>
+      </c>
+      <c r="L125" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="M125" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="127" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="128" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>

</xml_diff>

<commit_message>
data tong hop 18/9
</commit_message>
<xml_diff>
--- a/Thuthapdulieu.xlsx
+++ b/Thuthapdulieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mai\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F456795-4A99-40AF-98FB-4DCC2354AF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8673220-F018-4642-ACF4-4CE6C0D7596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29890" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="746">
   <si>
     <t>id</t>
   </si>
@@ -1900,13 +1900,376 @@
   </si>
   <si>
     <t>000124</t>
+  </si>
+  <si>
+    <t>biden-putin-16634297804681543076803.jpg</t>
+  </si>
+  <si>
+    <t>BLOOMBERG/GETTY IMAGES</t>
+  </si>
+  <si>
+    <t>Ông Biden cảnh báo ông Putin không dùng vũ khí hạt nhân ở Ukraine</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/17/biden-putin-16634297804681543076803.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-biden-canh-bao-ong-putin-khong-dung-vu-khi-hat-nhan-o-ukraine-20220917225035706.htm</t>
+  </si>
+  <si>
+    <t>thiếu ngày, sự kiện, ảnh ghép 2 nhân vật</t>
+  </si>
+  <si>
+    <t>putin-16634153003042021838443.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/17/putin-16634153003042021838443.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tass-81-5-nguoi-nga-tin-nhiem-tong-thong-putin-20220917190602129.htm</t>
+  </si>
+  <si>
+    <t>putin-modi-16633374117011843038950.jpg</t>
+  </si>
+  <si>
+    <t>Thủ tướng Ấn Độ Narendra Modi (trái) gặp Tổng thống Nga Vladimir Putin bên lề hội nghị thượng đỉnh của Tổ chức Hợp tác Thượng Hải (SCO) tại Uzbekistan, ngày 16-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/putin-modi-16633374117011843038950.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/doi-thoai-voi-thu-tuong-an-do-ong-putin-noi-muon-xung-dot-ukraine-ket-thuc-som-20220916211058647.htm</t>
+  </si>
+  <si>
+    <t>2022-09-16t090237z1472950776rc28iw9fntw6rtrmadp3uzbekistan-sco-16633193874952020983722.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/2022-09-16t090237z1472950776rc28iw9fntw6rtrmadp3uzbekistan-sco-16633193874952020983722.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tong-thong-putin-tuyen-bo-tang-300-000-tan-phan-bon-20220916161413368.htm</t>
+  </si>
+  <si>
+    <t>uzbekistan-sco-4read-only-16633481102301238714829.jpg</t>
+  </si>
+  <si>
+    <t>Lãnh đạo các nước thành viên Tổ chức Hợp tác Thượng Hải (SCO) trong một cuộc họp hẹp ở Samarkand, Uzbekistan, ngày 16-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/17/uzbekistan-sco-4read-only-16633481102301238714829.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/nga-trung-va-nhung-tam-the-khac-nhau-20220917003604683.htm</t>
+  </si>
+  <si>
+    <t>biden-2-16633471576071836883673.jpg</t>
+  </si>
+  <si>
+    <t>DPA</t>
+  </si>
+  <si>
+    <t>Đương kim Tổng thống Mỹ Joe Biden</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/16/biden-2-16633471576071836883673.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/6-tong-thong-my-gan-day-ai-giau-nhat-20220916234606334.htm</t>
+  </si>
+  <si>
+    <t>lat-chien-thu-trung-quoc-1662285289760149384546.png</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>SCMP</t>
+  </si>
+  <si>
+    <t>Ông Lật Chiến Thư (trái) trong cuộc gặp với Tổng thống Nga Vladimir Putin năm 2017 tại Điện Kremlin</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/4/lat-chien-thu-trung-quoc-1662285289760149384546.png</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/chu-tich-quoc-hoi-trung-quoc-sap-den-nga-20220904165957065.htm</t>
+  </si>
+  <si>
+    <t>trump-mittinh-16622674838821115138607.jpg</t>
+  </si>
+  <si>
+    <t>Cựu tổng thống Trump tại sự kiện ở Pennsylvania ngày 3-9</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/4/trump-mittinh-16622674838821115138607.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-trump-trut-gian-len-dang-dan-chu-tai-mit-tinh-cuu-nuoc-my-20220904115927123.htm</t>
+  </si>
+  <si>
+    <t>hoi-nghi-thuong-dinh-my-thai-binh-duong-1662128944840802877465.png</t>
+  </si>
+  <si>
+    <t>Kamala Harris</t>
+  </si>
+  <si>
+    <t>Phó Tổng thống Mỹ</t>
+  </si>
+  <si>
+    <t>diễn đàng các đảo quốc Thái Bình Dương</t>
+  </si>
+  <si>
+    <t>7/2022</t>
+  </si>
+  <si>
+    <t>trực tuyến</t>
+  </si>
+  <si>
+    <t>Phó tổng thống Mỹ Kamala Harris phát biểu tại Diễn đàn các đảo quốc Thái Bình Dương được tổ chức trực tuyến hồi giữa tháng 7-2022</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/2/hoi-nghi-thuong-dinh-my-thai-binh-duong-1662128944840802877465.png</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/my-tap-trung-canh-tranh-anh-huong-voi-trung-quoc-o-thai-binh-duong-20220902213123303.htm</t>
+  </si>
+  <si>
+    <t>pm9-tiep-ngoai-truong-my-01-nguyen-khanh-1652484085268591231563-1662088503312181048140.jpg</t>
+  </si>
+  <si>
+    <t>cuộc gặp ở Washington</t>
+  </si>
+  <si>
+    <t>5/2022</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Nguyễn Khánh</t>
+  </si>
+  <si>
+    <t>Thủ tướng Phạm Minh Chính tiếp Ngoại trưởng Mỹ Antony Blinken tại Washington vào tháng 5-2022</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/2/pm9-tiep-ngoai-truong-my-01-nguyen-khanh-1652484085268591231563-1662088503312181048140.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ngoai-truong-my-chuc-mung-quoc-khanh-viet-nam-20220902101752922.htm</t>
+  </si>
+  <si>
+    <t>tap-can-binh-166199263600228870229.jpg</t>
+  </si>
+  <si>
+    <t>đại hội Đảng toàn quốc</t>
+  </si>
+  <si>
+    <t>Chủ tịch Trung Quốc Tập Cận Bình (trung tâm) trong kỳ đại hội đảng toàn quốc năm 2017 tại Bắc Kinh</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/1/tap-can-binh-166199263600228870229.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/nhieu-du-doan-truoc-dai-hoi-dang-o-trung-quoc-20220901074120031.htm</t>
+  </si>
+  <si>
+    <t>biden-trump-fbi-16619072783161447054085.jpg</t>
+  </si>
+  <si>
+    <t>bài phát biểu và kế hoạch "Nước Mỹ an toàn hơn"</t>
+  </si>
+  <si>
+    <t>30/8/2022</t>
+  </si>
+  <si>
+    <t>Tổng thống Biden trong bài phát biểu về bạo lực súng đạn, quyền của cảnh sát và kế hoạch "Nước Mỹ an toàn hơn" tại Pennsylvania ngày 30-8</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/8/31/biden-trump-fbi-16619072783161447054085.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-biden-goi-nhung-nguoi-chi-trich-fbi-vi-kham-nha-ong-trump-la-benh-hoan-20220831075145378.htm</t>
+  </si>
+  <si>
+    <t>queen-1-1662662153701271213714.jpg</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth II mỉm cười khi đến dự sự kiện khánh thành Phòng thí nghiệm Sainsbury về nghiên cứu thực vật ở Đại học Vườn cây Cambridge (Anh) ngày 27-4-2011</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-1-1662662153701271213714.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/nu-hoang-elizabeth-ii-va-nhung-ky-luc-thu-vi-20220909013425398.htm</t>
+  </si>
+  <si>
+    <t>queen-5-1662662460161481409563.jpg</t>
+  </si>
+  <si>
+    <t>nữ hoàng đến Học viện Quân sự Hoàng gia ở Sandhurst</t>
+  </si>
+  <si>
+    <t>12/4/2006</t>
+  </si>
+  <si>
+    <t>Sandhurst</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth II mỉm cười khi đi ngang cháu nội là Hoàng tử Harry đứng trong hàng quân danh dự của Học viện Quân sự Hoàng gia ở Sandhurst, miền nam nước Anh, ngày 12-4-2006</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-5-1662662460161481409563.jpg</t>
+  </si>
+  <si>
+    <t>queen-2-16626619646711507346630.jpg</t>
+  </si>
+  <si>
+    <t>phát biểu khai mạc Quốc hội Anh</t>
+  </si>
+  <si>
+    <t>14/10/2019</t>
+  </si>
+  <si>
+    <t>Nữ hoàng Elizabeth II và Thái tử Charles, trong sự kiện Nữ hoàng phát biểu khai mạc Quốc hội Anh ở thủ đô London, ngày 14-10-2019.</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-2-16626619646711507346630.jpg</t>
+  </si>
+  <si>
+    <t>queen-6-1662663483443691101448.jpg</t>
+  </si>
+  <si>
+    <t>tiếp đón Tổng thống Mỹ Barack Obama</t>
+  </si>
+  <si>
+    <t>24/5/2011</t>
+  </si>
+  <si>
+    <t>Nữ hoàng tiếp đón Tổng thống Mỹ Barack Obama tại Điện Buckingham ở London, ngày 24-5-2011</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-6-1662663483443691101448.jpg</t>
+  </si>
+  <si>
+    <t>queen-7-16626639967851569339283.jpg</t>
+  </si>
+  <si>
+    <t>phát biểu tại Đại hội đồng Liên Hiệp Quốc</t>
+  </si>
+  <si>
+    <t>6/7/2010</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Nữ hoàng phát biểu tại Đại hội đồng Liên Hiệp Quốc ở trụ sở tại New York (Mỹ) vào ngày 6-7-2010</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-7-16626639967851569339283.jpg</t>
+  </si>
+  <si>
+    <t>queen-3-16626622834972080210638.jpg</t>
+  </si>
+  <si>
+    <t>khai màn một sự kiện ở Luân Đôn</t>
+  </si>
+  <si>
+    <t>12/6/2010</t>
+  </si>
+  <si>
+    <t>Nữ hoàng đến khai màn sự kiện ở London, ngày 12-6-2010</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-3-16626622834972080210638.jpg</t>
+  </si>
+  <si>
+    <t>queen-4-166266236721929178125.jpg</t>
+  </si>
+  <si>
+    <t>trở về Điện Buckingham sau khi dự đám cưới của cháu nội là Hoàng tử William với Kate Middleton</t>
+  </si>
+  <si>
+    <t>29/4/2011</t>
+  </si>
+  <si>
+    <t>Nữ hoàng và chồng là Hoàng thân Philip trên đường về Điện Buckingham sau khi dự đám cưới của cháu nội là Hoàng tử William với Kate Middleton ngày 29-4-2011</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/9/9/queen-4-166266236721929178125.jpg</t>
+  </si>
+  <si>
+    <t>000125</t>
+  </si>
+  <si>
+    <t>000126</t>
+  </si>
+  <si>
+    <t>000127</t>
+  </si>
+  <si>
+    <t>000128</t>
+  </si>
+  <si>
+    <t>000129</t>
+  </si>
+  <si>
+    <t>000130</t>
+  </si>
+  <si>
+    <t>000131</t>
+  </si>
+  <si>
+    <t>000132</t>
+  </si>
+  <si>
+    <t>000133</t>
+  </si>
+  <si>
+    <t>000134</t>
+  </si>
+  <si>
+    <t>000135</t>
+  </si>
+  <si>
+    <t>000136</t>
+  </si>
+  <si>
+    <t>000137</t>
+  </si>
+  <si>
+    <t>000138</t>
+  </si>
+  <si>
+    <t>000139</t>
+  </si>
+  <si>
+    <t>000140</t>
+  </si>
+  <si>
+    <t>000141</t>
+  </si>
+  <si>
+    <t>000142</t>
+  </si>
+  <si>
+    <t>000143</t>
+  </si>
+  <si>
+    <t>000144</t>
+  </si>
+  <si>
+    <t>000145</t>
+  </si>
+  <si>
+    <t>000146</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1984,6 +2347,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2025,7 +2394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2056,6 +2425,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2277,8 +2648,8 @@
   </sheetPr>
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -6582,7 +6953,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="113" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A113" s="6" t="s">
         <v>612</v>
       </c>
@@ -6620,7 +6991,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="114" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A114" s="6" t="s">
         <v>613</v>
       </c>
@@ -6658,7 +7029,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="115" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A115" s="6" t="s">
         <v>614</v>
       </c>
@@ -6696,7 +7067,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="116" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A116" s="6" t="s">
         <v>615</v>
       </c>
@@ -6734,7 +7105,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="117" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A117" s="6" t="s">
         <v>616</v>
       </c>
@@ -6772,7 +7143,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="118" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="118" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A118" s="6" t="s">
         <v>617</v>
       </c>
@@ -6810,7 +7181,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="119" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A119" s="6" t="s">
         <v>618</v>
       </c>
@@ -6848,7 +7219,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="120" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A120" s="6" t="s">
         <v>619</v>
       </c>
@@ -6886,7 +7257,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="121" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A121" s="6" t="s">
         <v>620</v>
       </c>
@@ -6924,7 +7295,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="122" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A122" s="6" t="s">
         <v>621</v>
       </c>
@@ -6962,7 +7333,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="123" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A123" s="6" t="s">
         <v>622</v>
       </c>
@@ -7000,7 +7371,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="124" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A124" s="6" t="s">
         <v>623</v>
       </c>
@@ -7038,7 +7409,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="125" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A125" s="6" t="s">
         <v>624</v>
       </c>
@@ -7076,41 +7447,834 @@
         <v>594</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="127" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="128" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="126" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A126" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J126" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="K126" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="L126" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="M126" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="N126" s="14" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A127" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="J127" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="K127" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="L127" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="M127" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="N127" s="14" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A128" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F128" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G128" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H128" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J128" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="K128" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="L128" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="M128" s="14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A129" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="C129" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F129" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G129" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H129" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J129" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K129" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="L129" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="M129" s="14" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A130" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F130" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G130" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H130" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J130" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K130" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="L130" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="M130" s="14" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A131" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D131" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F131" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="G131" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H131" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J131" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K131" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="L131" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="M131" s="14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A132" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="C132" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D132" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F132" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="G132" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H132" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="J132" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K132" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="L132" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="M132" s="14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A133" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>645</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D133" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J133" s="10" t="s">
+        <v>646</v>
+      </c>
+      <c r="K133" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="L133" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="M133" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="N133" s="17" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A134" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>650</v>
+      </c>
+      <c r="C134" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D134" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F134" s="30" t="s">
+        <v>651</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J134" s="16" t="s">
+        <v>652</v>
+      </c>
+      <c r="K134" s="14" t="s">
+        <v>653</v>
+      </c>
+      <c r="L134" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="M134" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="N134" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A135" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>656</v>
+      </c>
+      <c r="C135" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E135" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F135" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J135" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K135" s="14" t="s">
+        <v>657</v>
+      </c>
+      <c r="L135" s="14" t="s">
+        <v>658</v>
+      </c>
+      <c r="M135" s="14" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A136" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>660</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="D136" s="16" t="s">
+        <v>662</v>
+      </c>
+      <c r="E136" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="F136" s="30" t="s">
+        <v>664</v>
+      </c>
+      <c r="G136" s="31" t="s">
+        <v>665</v>
+      </c>
+      <c r="J136" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K136" s="14" t="s">
+        <v>666</v>
+      </c>
+      <c r="L136" s="14" t="s">
+        <v>667</v>
+      </c>
+      <c r="M136" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="N136" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A137" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>669</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D137" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E137" s="14" t="s">
+        <v>670</v>
+      </c>
+      <c r="F137" s="30" t="s">
+        <v>671</v>
+      </c>
+      <c r="G137" s="31" t="s">
+        <v>672</v>
+      </c>
+      <c r="H137" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="I137" s="31" t="s">
+        <v>673</v>
+      </c>
+      <c r="K137" s="14" t="s">
+        <v>674</v>
+      </c>
+      <c r="L137" s="14" t="s">
+        <v>675</v>
+      </c>
+      <c r="M137" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="N137" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A138" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>677</v>
+      </c>
+      <c r="C138" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D138" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E138" s="14" t="s">
+        <v>678</v>
+      </c>
+      <c r="F138" s="30" t="s">
+        <v>651</v>
+      </c>
+      <c r="G138" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="H138" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="J138" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="K138" s="14" t="s">
+        <v>679</v>
+      </c>
+      <c r="L138" s="14" t="s">
+        <v>680</v>
+      </c>
+      <c r="M138" s="14" t="s">
+        <v>681</v>
+      </c>
+      <c r="N138" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A139" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>682</v>
+      </c>
+      <c r="C139" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E139" s="14" t="s">
+        <v>683</v>
+      </c>
+      <c r="F139" s="30" t="s">
+        <v>684</v>
+      </c>
+      <c r="G139" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="H139" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J139" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K139" s="14" t="s">
+        <v>685</v>
+      </c>
+      <c r="L139" s="14" t="s">
+        <v>686</v>
+      </c>
+      <c r="M139" s="14" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A140" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>688</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D140" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E140" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="F140" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="G140" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="H140" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J140" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K140" s="14" t="s">
+        <v>689</v>
+      </c>
+      <c r="L140" s="14" t="s">
+        <v>690</v>
+      </c>
+      <c r="M140" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A141" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>692</v>
+      </c>
+      <c r="C141" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D141" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E141" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="F141" s="30" t="s">
+        <v>694</v>
+      </c>
+      <c r="G141" s="16" t="s">
+        <v>695</v>
+      </c>
+      <c r="H141" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J141" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K141" s="14" t="s">
+        <v>696</v>
+      </c>
+      <c r="L141" s="14" t="s">
+        <v>697</v>
+      </c>
+      <c r="M141" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A142" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="C142" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D142" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E142" s="14" t="s">
+        <v>699</v>
+      </c>
+      <c r="F142" s="30" t="s">
+        <v>700</v>
+      </c>
+      <c r="G142" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H142" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J142" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K142" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="L142" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="M142" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A143" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D143" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E143" s="14" t="s">
+        <v>699</v>
+      </c>
+      <c r="F143" s="30" t="s">
+        <v>700</v>
+      </c>
+      <c r="G143" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H143" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J143" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K143" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="L143" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="M143" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A144" s="6" t="s">
+        <v>742</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>703</v>
+      </c>
+      <c r="C144" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D144" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E144" s="14" t="s">
+        <v>704</v>
+      </c>
+      <c r="F144" s="30" t="s">
+        <v>705</v>
+      </c>
+      <c r="G144" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H144" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J144" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K144" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="L144" s="14" t="s">
+        <v>707</v>
+      </c>
+      <c r="M144" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A145" s="6" t="s">
+        <v>743</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>708</v>
+      </c>
+      <c r="C145" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D145" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E145" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="F145" s="30" t="s">
+        <v>710</v>
+      </c>
+      <c r="G145" s="16" t="s">
+        <v>711</v>
+      </c>
+      <c r="H145" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J145" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K145" s="14" t="s">
+        <v>712</v>
+      </c>
+      <c r="L145" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="M145" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A146" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>714</v>
+      </c>
+      <c r="C146" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D146" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E146" s="14" t="s">
+        <v>715</v>
+      </c>
+      <c r="F146" s="30" t="s">
+        <v>716</v>
+      </c>
+      <c r="G146" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H146" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J146" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K146" s="14" t="s">
+        <v>717</v>
+      </c>
+      <c r="L146" s="14" t="s">
+        <v>718</v>
+      </c>
+      <c r="M146" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A147" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="B147" s="14" t="s">
+        <v>719</v>
+      </c>
+      <c r="C147" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="E147" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="F147" s="30" t="s">
+        <v>721</v>
+      </c>
+      <c r="G147" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H147" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J147" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K147" s="14" t="s">
+        <v>722</v>
+      </c>
+      <c r="L147" s="14" t="s">
+        <v>723</v>
+      </c>
+      <c r="M147" s="14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="149" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="150" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="151" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="152" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="153" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="154" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="155" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="156" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="157" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="158" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="159" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="160" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -7952,6 +9116,26 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="M31:N31"/>
@@ -7962,26 +9146,6 @@
     <mergeCell ref="M27:N27"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>

</xml_diff>